<commit_message>
renamed data files to support use in R
</commit_message>
<xml_diff>
--- a/Data/Gratitude.xlsx
+++ b/Data/Gratitude.xlsx
@@ -1,23 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ghsaund/Documents/GitHub/BYUI_M221_Book_R/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Downloads\Temp data folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D26F566C-24DC-2340-9ECB-65377D0D706D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129F94FE-7DBD-4024-AED0-39CE5F648205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="17900" windowHeight="13580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -31,9 +42,6 @@
   </si>
   <si>
     <t>Events</t>
-  </si>
-  <si>
-    <t>Source</t>
   </si>
   <si>
     <t>Data representative of values reported in Table 2 of the paper:</t>
@@ -69,13 +77,16 @@
     <t>Higher scores indicate a more favorable disposition to life in general.</t>
   </si>
   <si>
-    <t>Treatment Group</t>
+    <t>person</t>
   </si>
   <si>
-    <t>Happiness Score</t>
+    <t>treatment group</t>
   </si>
   <si>
-    <t>Person</t>
+    <t>happiness score</t>
+  </si>
+  <si>
+    <t>source</t>
   </si>
 </sst>
 </file>
@@ -454,14 +465,14 @@
   <dimension ref="A1:D193"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A192" sqref="A192"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
         <v>15</v>
@@ -470,10 +481,10 @@
         <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -484,10 +495,10 @@
         <v>6.1</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -498,10 +509,10 @@
         <v>6.2</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -512,10 +523,10 @@
         <v>3.7</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -526,10 +537,10 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -540,10 +551,10 @@
         <v>5.7</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -554,10 +565,10 @@
         <v>7.5</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -568,10 +579,10 @@
         <v>5.4</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -582,10 +593,10 @@
         <v>4.3</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -596,10 +607,10 @@
         <v>4.8</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -610,10 +621,10 @@
         <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -624,10 +635,10 @@
         <v>5.6</v>
       </c>
       <c r="D12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -638,10 +649,10 @@
         <v>4.3</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -652,10 +663,10 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -666,10 +677,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -680,10 +691,10 @@
         <v>3.9</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -694,10 +705,10 @@
         <v>5.2</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -708,10 +719,10 @@
         <v>4.2</v>
       </c>
       <c r="D18" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -722,10 +733,10 @@
         <v>6</v>
       </c>
       <c r="D19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -736,10 +747,10 @@
         <v>5.7</v>
       </c>
       <c r="D20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -750,10 +761,10 @@
         <v>3.5</v>
       </c>
       <c r="D21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -764,10 +775,10 @@
         <v>6.6</v>
       </c>
       <c r="D22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -778,10 +789,10 @@
         <v>5.8</v>
       </c>
       <c r="D23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -792,10 +803,10 @@
         <v>5.3</v>
       </c>
       <c r="D24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -806,10 +817,10 @@
         <v>3.9</v>
       </c>
       <c r="D25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -820,10 +831,10 @@
         <v>5</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -834,10 +845,10 @@
         <v>3.8</v>
       </c>
       <c r="D27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -848,10 +859,10 @@
         <v>4.3</v>
       </c>
       <c r="D28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -862,10 +873,10 @@
         <v>5</v>
       </c>
       <c r="D29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -876,10 +887,10 @@
         <v>5.7</v>
       </c>
       <c r="D30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -890,10 +901,10 @@
         <v>5.4</v>
       </c>
       <c r="D31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -904,10 +915,10 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -918,10 +929,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -932,10 +943,10 @@
         <v>5.5</v>
       </c>
       <c r="D34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -946,10 +957,10 @@
         <v>6.2</v>
       </c>
       <c r="D35" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -960,10 +971,10 @@
         <v>6.2</v>
       </c>
       <c r="D36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -974,10 +985,10 @@
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
@@ -988,10 +999,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D38" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1002,10 +1013,10 @@
         <v>6.6</v>
       </c>
       <c r="D39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1016,10 +1027,10 @@
         <v>5.5</v>
       </c>
       <c r="D40" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1030,10 +1041,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D41" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1044,10 +1055,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D42" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1058,10 +1069,10 @@
         <v>5.3</v>
       </c>
       <c r="D43" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1072,10 +1083,10 @@
         <v>4.3</v>
       </c>
       <c r="D44" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1086,10 +1097,10 @@
         <v>3.5</v>
       </c>
       <c r="D45" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1100,10 +1111,10 @@
         <v>5.6</v>
       </c>
       <c r="D46" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1114,10 +1125,10 @@
         <v>3.8</v>
       </c>
       <c r="D47" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1128,10 +1139,10 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="D48" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1142,10 +1153,10 @@
         <v>4</v>
       </c>
       <c r="D49" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1156,10 +1167,10 @@
         <v>7</v>
       </c>
       <c r="D50" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1170,10 +1181,10 @@
         <v>7.2</v>
       </c>
       <c r="D51" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1184,10 +1195,10 @@
         <v>4.2</v>
       </c>
       <c r="D52" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1198,10 +1209,10 @@
         <v>4.2</v>
       </c>
       <c r="D53" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1212,10 +1223,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D54" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1226,10 +1237,10 @@
         <v>4.2</v>
       </c>
       <c r="D55" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1240,10 +1251,10 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D56" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1254,10 +1265,10 @@
         <v>5.4</v>
       </c>
       <c r="D57" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1268,10 +1279,10 @@
         <v>5</v>
       </c>
       <c r="D58" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1282,10 +1293,10 @@
         <v>6.5</v>
       </c>
       <c r="D59" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1296,10 +1307,10 @@
         <v>4.8</v>
       </c>
       <c r="D60" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1310,10 +1321,10 @@
         <v>4</v>
       </c>
       <c r="D61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1324,10 +1335,10 @@
         <v>5.3</v>
       </c>
       <c r="D62" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1338,10 +1349,10 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="D63" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1352,10 +1363,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D64" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1366,10 +1377,10 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D65" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1380,10 +1391,10 @@
         <v>5.9</v>
       </c>
       <c r="D66" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1394,10 +1405,10 @@
         <v>5.4</v>
       </c>
       <c r="D67" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1408,10 +1419,10 @@
         <v>3.7</v>
       </c>
       <c r="D68" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1422,10 +1433,10 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="D69" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1436,10 +1447,10 @@
         <v>3.8</v>
       </c>
       <c r="D70" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1450,10 +1461,10 @@
         <v>3.4</v>
       </c>
       <c r="D71" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>71</v>
       </c>
@@ -1464,10 +1475,10 @@
         <v>5.3</v>
       </c>
       <c r="D72" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>72</v>
       </c>
@@ -1478,10 +1489,10 @@
         <v>5.4</v>
       </c>
       <c r="D73" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>73</v>
       </c>
@@ -1492,10 +1503,10 @@
         <v>4.2</v>
       </c>
       <c r="D74" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>74</v>
       </c>
@@ -1506,10 +1517,10 @@
         <v>5.5</v>
       </c>
       <c r="D75" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>75</v>
       </c>
@@ -1520,10 +1531,10 @@
         <v>6.1</v>
       </c>
       <c r="D76" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>76</v>
       </c>
@@ -1534,10 +1545,10 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="D77" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>77</v>
       </c>
@@ -1548,10 +1559,10 @@
         <v>6.2</v>
       </c>
       <c r="D78" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>78</v>
       </c>
@@ -1562,10 +1573,10 @@
         <v>3.9</v>
       </c>
       <c r="D79" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>79</v>
       </c>
@@ -1576,10 +1587,10 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="D80" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>80</v>
       </c>
@@ -1590,10 +1601,10 @@
         <v>3.4</v>
       </c>
       <c r="D81" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>81</v>
       </c>
@@ -1604,10 +1615,10 @@
         <v>5.3</v>
       </c>
       <c r="D82" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>82</v>
       </c>
@@ -1618,10 +1629,10 @@
         <v>3.7</v>
       </c>
       <c r="D83" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>83</v>
       </c>
@@ -1632,10 +1643,10 @@
         <v>4.5</v>
       </c>
       <c r="D84" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>84</v>
       </c>
@@ -1646,10 +1657,10 @@
         <v>4.2</v>
       </c>
       <c r="D85" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>85</v>
       </c>
@@ -1660,10 +1671,10 @@
         <v>3.5</v>
       </c>
       <c r="D86" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>86</v>
       </c>
@@ -1674,10 +1685,10 @@
         <v>3.5</v>
       </c>
       <c r="D87" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>87</v>
       </c>
@@ -1688,10 +1699,10 @@
         <v>5.2</v>
       </c>
       <c r="D88" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>88</v>
       </c>
@@ -1702,10 +1713,10 @@
         <v>5.9</v>
       </c>
       <c r="D89" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>89</v>
       </c>
@@ -1716,10 +1727,10 @@
         <v>5.9</v>
       </c>
       <c r="D90" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>90</v>
       </c>
@@ -1730,10 +1741,10 @@
         <v>4.5</v>
       </c>
       <c r="D91" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>91</v>
       </c>
@@ -1744,10 +1755,10 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="D92" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>92</v>
       </c>
@@ -1758,10 +1769,10 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="D93" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>93</v>
       </c>
@@ -1772,10 +1783,10 @@
         <v>6</v>
       </c>
       <c r="D94" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>94</v>
       </c>
@@ -1786,10 +1797,10 @@
         <v>3.8</v>
       </c>
       <c r="D95" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>95</v>
       </c>
@@ -1800,10 +1811,10 @@
         <v>4.7</v>
       </c>
       <c r="D96" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>96</v>
       </c>
@@ -1814,10 +1825,10 @@
         <v>5.4</v>
       </c>
       <c r="D97" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>97</v>
       </c>
@@ -1828,10 +1839,10 @@
         <v>3.5</v>
       </c>
       <c r="D98" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>98</v>
       </c>
@@ -1842,10 +1853,10 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="D99" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>99</v>
       </c>
@@ -1856,10 +1867,10 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="D100" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>100</v>
       </c>
@@ -1870,10 +1881,10 @@
         <v>4.3</v>
       </c>
       <c r="D101" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>101</v>
       </c>
@@ -1884,10 +1895,10 @@
         <v>4.7</v>
       </c>
       <c r="D102" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>102</v>
       </c>
@@ -1898,10 +1909,10 @@
         <v>3.8</v>
       </c>
       <c r="D103" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>103</v>
       </c>
@@ -1912,10 +1923,10 @@
         <v>5.3</v>
       </c>
       <c r="D104" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>104</v>
       </c>
@@ -1926,10 +1937,10 @@
         <v>3.9</v>
       </c>
       <c r="D105" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>105</v>
       </c>
@@ -1940,10 +1951,10 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="D106" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>106</v>
       </c>
@@ -1954,10 +1965,10 @@
         <v>3.3</v>
       </c>
       <c r="D107" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>107</v>
       </c>
@@ -1968,10 +1979,10 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="D108" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>108</v>
       </c>
@@ -1982,10 +1993,10 @@
         <v>3.4</v>
       </c>
       <c r="D109" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>109</v>
       </c>
@@ -1996,10 +2007,10 @@
         <v>4.8</v>
       </c>
       <c r="D110" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>110</v>
       </c>
@@ -2010,10 +2021,10 @@
         <v>5.6</v>
       </c>
       <c r="D111" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>111</v>
       </c>
@@ -2024,10 +2035,10 @@
         <v>3.8</v>
       </c>
       <c r="D112" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>112</v>
       </c>
@@ -2038,10 +2049,10 @@
         <v>5.6</v>
       </c>
       <c r="D113" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>113</v>
       </c>
@@ -2052,10 +2063,10 @@
         <v>4.8</v>
       </c>
       <c r="D114" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>114</v>
       </c>
@@ -2066,10 +2077,10 @@
         <v>4.7</v>
       </c>
       <c r="D115" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>115</v>
       </c>
@@ -2080,10 +2091,10 @@
         <v>5.4</v>
       </c>
       <c r="D116" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>116</v>
       </c>
@@ -2094,10 +2105,10 @@
         <v>4.8</v>
       </c>
       <c r="D117" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>117</v>
       </c>
@@ -2108,10 +2119,10 @@
         <v>5.6</v>
       </c>
       <c r="D118" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>118</v>
       </c>
@@ -2122,10 +2133,10 @@
         <v>4.8</v>
       </c>
       <c r="D119" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>119</v>
       </c>
@@ -2136,10 +2147,10 @@
         <v>5.5</v>
       </c>
       <c r="D120" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>120</v>
       </c>
@@ -2150,10 +2161,10 @@
         <v>5.3</v>
       </c>
       <c r="D121" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>121</v>
       </c>
@@ -2164,10 +2175,10 @@
         <v>5.6</v>
       </c>
       <c r="D122" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>122</v>
       </c>
@@ -2178,10 +2189,10 @@
         <v>3.7</v>
       </c>
       <c r="D123" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>123</v>
       </c>
@@ -2192,10 +2203,10 @@
         <v>3.8</v>
       </c>
       <c r="D124" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>124</v>
       </c>
@@ -2206,10 +2217,10 @@
         <v>5.3</v>
       </c>
       <c r="D125" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>125</v>
       </c>
@@ -2220,10 +2231,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D126" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>126</v>
       </c>
@@ -2234,10 +2245,10 @@
         <v>6.2</v>
       </c>
       <c r="D127" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>127</v>
       </c>
@@ -2248,10 +2259,10 @@
         <v>3.8</v>
       </c>
       <c r="D128" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>128</v>
       </c>
@@ -2262,10 +2273,10 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D129" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>129</v>
       </c>
@@ -2276,10 +2287,10 @@
         <v>4.2</v>
       </c>
       <c r="D130" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>130</v>
       </c>
@@ -2290,10 +2301,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D131" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>131</v>
       </c>
@@ -2304,10 +2315,10 @@
         <v>4.8</v>
       </c>
       <c r="D132" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>132</v>
       </c>
@@ -2318,10 +2329,10 @@
         <v>6.7</v>
       </c>
       <c r="D133" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>133</v>
       </c>
@@ -2332,10 +2343,10 @@
         <v>3.6</v>
       </c>
       <c r="D134" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>134</v>
       </c>
@@ -2346,10 +2357,10 @@
         <v>4.8</v>
       </c>
       <c r="D135" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>135</v>
       </c>
@@ -2360,10 +2371,10 @@
         <v>4.7</v>
       </c>
       <c r="D136" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>136</v>
       </c>
@@ -2374,10 +2385,10 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="D137" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>137</v>
       </c>
@@ -2388,10 +2399,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D138" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>138</v>
       </c>
@@ -2402,10 +2413,10 @@
         <v>5.4</v>
       </c>
       <c r="D139" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>139</v>
       </c>
@@ -2416,10 +2427,10 @@
         <v>4</v>
       </c>
       <c r="D140" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>140</v>
       </c>
@@ -2430,10 +2441,10 @@
         <v>3.8</v>
       </c>
       <c r="D141" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>141</v>
       </c>
@@ -2444,10 +2455,10 @@
         <v>4.5</v>
       </c>
       <c r="D142" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>142</v>
       </c>
@@ -2458,10 +2469,10 @@
         <v>5.2</v>
       </c>
       <c r="D143" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>143</v>
       </c>
@@ -2472,10 +2483,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D144" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>144</v>
       </c>
@@ -2486,10 +2497,10 @@
         <v>4.5</v>
       </c>
       <c r="D145" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="146" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>145</v>
       </c>
@@ -2500,10 +2511,10 @@
         <v>3</v>
       </c>
       <c r="D146" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="147" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>146</v>
       </c>
@@ -2514,10 +2525,10 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D147" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>147</v>
       </c>
@@ -2528,10 +2539,10 @@
         <v>4.2</v>
       </c>
       <c r="D148" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="149" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>148</v>
       </c>
@@ -2542,10 +2553,10 @@
         <v>3.9</v>
       </c>
       <c r="D149" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="150" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>149</v>
       </c>
@@ -2556,10 +2567,10 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D150" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="151" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>150</v>
       </c>
@@ -2570,10 +2581,10 @@
         <v>5.2</v>
       </c>
       <c r="D151" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="152" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>151</v>
       </c>
@@ -2584,10 +2595,10 @@
         <v>3.3</v>
       </c>
       <c r="D152" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="153" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>152</v>
       </c>
@@ -2598,10 +2609,10 @@
         <v>4.7</v>
       </c>
       <c r="D153" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>153</v>
       </c>
@@ -2612,10 +2623,10 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D154" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="155" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>154</v>
       </c>
@@ -2626,10 +2637,10 @@
         <v>5</v>
       </c>
       <c r="D155" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>155</v>
       </c>
@@ -2640,10 +2651,10 @@
         <v>4.3</v>
       </c>
       <c r="D156" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>156</v>
       </c>
@@ -2654,10 +2665,10 @@
         <v>4.7</v>
       </c>
       <c r="D157" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>157</v>
       </c>
@@ -2668,10 +2679,10 @@
         <v>4.2</v>
       </c>
       <c r="D158" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>158</v>
       </c>
@@ -2682,10 +2693,10 @@
         <v>5.5</v>
       </c>
       <c r="D159" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="160" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>159</v>
       </c>
@@ -2696,10 +2707,10 @@
         <v>4.3</v>
       </c>
       <c r="D160" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="161" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>160</v>
       </c>
@@ -2710,10 +2721,10 @@
         <v>5.3</v>
       </c>
       <c r="D161" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="162" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>161</v>
       </c>
@@ -2724,10 +2735,10 @@
         <v>5</v>
       </c>
       <c r="D162" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="163" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>162</v>
       </c>
@@ -2738,10 +2749,10 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="D163" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="164" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>163</v>
       </c>
@@ -2752,10 +2763,10 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="D164" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="165" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>164</v>
       </c>
@@ -2766,10 +2777,10 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="D165" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="166" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>165</v>
       </c>
@@ -2780,10 +2791,10 @@
         <v>5.4</v>
       </c>
       <c r="D166" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="167" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>166</v>
       </c>
@@ -2794,10 +2805,10 @@
         <v>3.2</v>
       </c>
       <c r="D167" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="168" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>167</v>
       </c>
@@ -2808,10 +2819,10 @@
         <v>5</v>
       </c>
       <c r="D168" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="169" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>168</v>
       </c>
@@ -2822,10 +2833,10 @@
         <v>4.3</v>
       </c>
       <c r="D169" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="170" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>169</v>
       </c>
@@ -2836,10 +2847,10 @@
         <v>5.4</v>
       </c>
       <c r="D170" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="171" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>170</v>
       </c>
@@ -2850,10 +2861,10 @@
         <v>5</v>
       </c>
       <c r="D171" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="172" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>171</v>
       </c>
@@ -2864,10 +2875,10 @@
         <v>4.2</v>
       </c>
       <c r="D172" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="173" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>172</v>
       </c>
@@ -2878,10 +2889,10 @@
         <v>4</v>
       </c>
       <c r="D173" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>173</v>
       </c>
@@ -2892,10 +2903,10 @@
         <v>4.8</v>
       </c>
       <c r="D174" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>174</v>
       </c>
@@ -2906,10 +2917,10 @@
         <v>3.4</v>
       </c>
       <c r="D175" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="176" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>175</v>
       </c>
@@ -2920,10 +2931,10 @@
         <v>3.4</v>
       </c>
       <c r="D176" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="177" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>176</v>
       </c>
@@ -2934,10 +2945,10 @@
         <v>5.7</v>
       </c>
       <c r="D177" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="178" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>177</v>
       </c>
@@ -2948,10 +2959,10 @@
         <v>6.8</v>
       </c>
       <c r="D178" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="179" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>178</v>
       </c>
@@ -2962,10 +2973,10 @@
         <v>3.6</v>
       </c>
       <c r="D179" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="180" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>179</v>
       </c>
@@ -2976,10 +2987,10 @@
         <v>3.8</v>
       </c>
       <c r="D180" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="181" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>180</v>
       </c>
@@ -2990,10 +3001,10 @@
         <v>4.8</v>
       </c>
       <c r="D181" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="182" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>181</v>
       </c>
@@ -3004,10 +3015,10 @@
         <v>3.5</v>
       </c>
       <c r="D182" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="183" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>182</v>
       </c>
@@ -3018,10 +3029,10 @@
         <v>4.8</v>
       </c>
       <c r="D183" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="184" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>183</v>
       </c>
@@ -3032,10 +3043,10 @@
         <v>4.3</v>
       </c>
       <c r="D184" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="185" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>184</v>
       </c>
@@ -3046,10 +3057,10 @@
         <v>6</v>
       </c>
       <c r="D185" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="186" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A186">
         <v>185</v>
       </c>
@@ -3060,10 +3071,10 @@
         <v>6.7</v>
       </c>
       <c r="D186" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="187" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>186</v>
       </c>
@@ -3074,10 +3085,10 @@
         <v>5.7</v>
       </c>
       <c r="D187" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="188" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A188">
         <v>187</v>
       </c>
@@ -3088,10 +3099,10 @@
         <v>5.9</v>
       </c>
       <c r="D188" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="189" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>188</v>
       </c>
@@ -3102,10 +3113,10 @@
         <v>3.3</v>
       </c>
       <c r="D189" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="190" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>189</v>
       </c>
@@ -3116,10 +3127,10 @@
         <v>5.9</v>
       </c>
       <c r="D190" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="191" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>190</v>
       </c>
@@ -3130,10 +3141,10 @@
         <v>4.5</v>
       </c>
       <c r="D191" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="192" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>191</v>
       </c>
@@ -3144,10 +3155,10 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="D192" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="193" spans="1:4" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>192</v>
       </c>
@@ -3158,7 +3169,7 @@
         <v>3.7</v>
       </c>
       <c r="D193" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -3172,7 +3183,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3184,7 +3195,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revised data files and knitted additional lessons
</commit_message>
<xml_diff>
--- a/Data/Gratitude.xlsx
+++ b/Data/Gratitude.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Downloads\Temp data folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\craigaj\Documents\GitHub\M221R\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129F94FE-7DBD-4024-AED0-39CE5F648205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1706CEF5-6559-4C61-B2C4-8EC92AD47B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1370" yWindow="2830" windowWidth="14400" windowHeight="7370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,13 +80,13 @@
     <t>person</t>
   </si>
   <si>
-    <t>treatment group</t>
+    <t>happiness</t>
   </si>
   <si>
-    <t>happiness score</t>
+    <t>comments</t>
   </si>
   <si>
-    <t>source</t>
+    <t>treatment</t>
   </si>
 </sst>
 </file>
@@ -464,9 +464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -475,13 +473,13 @@
         <v>14</v>
       </c>
       <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>16</v>
-      </c>
-      <c r="D1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>